<commit_message>
templates und routes (authentication)
</commit_message>
<xml_diff>
--- a/models/stashedTrainData.XLSX
+++ b/models/stashedTrainData.XLSX
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="115">
   <si>
     <t>Produktmerkmal</t>
   </si>
@@ -47,6 +47,318 @@
   </si>
   <si>
     <t>Lenkungsmethode</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>1020</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>160</t>
+  </si>
+  <si>
+    <t>190</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>230</t>
+  </si>
+  <si>
+    <t>240</t>
+  </si>
+  <si>
+    <t>260</t>
+  </si>
+  <si>
+    <t>270</t>
+  </si>
+  <si>
+    <t>280</t>
+  </si>
+  <si>
+    <t>290</t>
+  </si>
+  <si>
+    <t>300</t>
+  </si>
+  <si>
+    <t>310</t>
+  </si>
+  <si>
+    <t>312</t>
+  </si>
+  <si>
+    <t>318</t>
+  </si>
+  <si>
+    <t>319</t>
+  </si>
+  <si>
+    <t>322</t>
+  </si>
+  <si>
+    <t>323</t>
+  </si>
+  <si>
+    <t>326</t>
+  </si>
+  <si>
+    <t>328</t>
+  </si>
+  <si>
+    <t>329</t>
+  </si>
+  <si>
+    <t>330</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>Rautiefe</t>
+  </si>
+  <si>
+    <t>Maschinenabnahme</t>
+  </si>
+  <si>
+    <t>siehe</t>
+  </si>
+  <si>
+    <t>Abstand</t>
+  </si>
+  <si>
+    <t>Rundheit</t>
+  </si>
+  <si>
+    <t>Zylinderform</t>
+  </si>
+  <si>
+    <t>Rundlauf</t>
+  </si>
+  <si>
+    <t>Bohrungs-ø</t>
+  </si>
+  <si>
+    <t>Bohrungstiefe</t>
+  </si>
+  <si>
+    <t>Innen-ø33,46</t>
+  </si>
+  <si>
+    <t>Innen-ø33,6H6</t>
+  </si>
+  <si>
+    <t>Innen-ø33,6</t>
+  </si>
+  <si>
+    <t>Aussen-ø37,4</t>
+  </si>
+  <si>
+    <t>Drehm.</t>
+  </si>
+  <si>
+    <t>Rolliertiefe</t>
+  </si>
+  <si>
+    <t>Sichtprüfung</t>
+  </si>
+  <si>
+    <t>0,000 µm</t>
+  </si>
+  <si>
+    <t>5,000 mm</t>
+  </si>
+  <si>
+    <t>3,000 mm</t>
+  </si>
+  <si>
+    <t>1,000 mm</t>
+  </si>
+  <si>
+    <t>0,000 mm</t>
+  </si>
+  <si>
+    <t>9,000 mm</t>
+  </si>
+  <si>
+    <t>33,600 mm</t>
+  </si>
+  <si>
+    <t>43,500 mm</t>
+  </si>
+  <si>
+    <t>48,500 mm</t>
+  </si>
+  <si>
+    <t>37,400 mm</t>
+  </si>
+  <si>
+    <t>10,000 mm</t>
+  </si>
+  <si>
+    <t>35,000 mm</t>
+  </si>
+  <si>
+    <t>16.0</t>
+  </si>
+  <si>
+    <t>30.0</t>
+  </si>
+  <si>
+    <t>5.5</t>
+  </si>
+  <si>
+    <t>10.0</t>
+  </si>
+  <si>
+    <t>3.1</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>0.005</t>
+  </si>
+  <si>
+    <t>0.015</t>
+  </si>
+  <si>
+    <t>0.05</t>
+  </si>
+  <si>
+    <t>12.5</t>
+  </si>
+  <si>
+    <t>25.0</t>
+  </si>
+  <si>
+    <t>9.0</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>33.616</t>
+  </si>
+  <si>
+    <t>43.525</t>
+  </si>
+  <si>
+    <t>48.6</t>
+  </si>
+  <si>
+    <t>37.45</t>
+  </si>
+  <si>
+    <t>10.6</t>
+  </si>
+  <si>
+    <t>35.0</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>5.0</t>
+  </si>
+  <si>
+    <t>3.0</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>8.9</t>
+  </si>
+  <si>
+    <t>33.604</t>
+  </si>
+  <si>
+    <t>43.475</t>
+  </si>
+  <si>
+    <t>48.4</t>
+  </si>
+  <si>
+    <t>37.4</t>
+  </si>
+  <si>
+    <t>9.4</t>
+  </si>
+  <si>
+    <t>34.8</t>
+  </si>
+  <si>
+    <t>µm</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>Drehen Komplett</t>
+  </si>
+  <si>
+    <t>MS40-MGH</t>
+  </si>
+  <si>
+    <t>Rauhigkeitsmessgerät</t>
+  </si>
+  <si>
+    <t>visuelle Prüfung</t>
+  </si>
+  <si>
+    <t>MESSUHR</t>
+  </si>
+  <si>
+    <t>MESSMASCHINE</t>
+  </si>
+  <si>
+    <t>Prüfhülse</t>
+  </si>
+  <si>
+    <t>1/444</t>
+  </si>
+  <si>
+    <t>1/1</t>
+  </si>
+  <si>
+    <t>2/20</t>
+  </si>
+  <si>
+    <t>6/120</t>
+  </si>
+  <si>
+    <t>2/30</t>
+  </si>
+  <si>
+    <t>1/60</t>
+  </si>
+  <si>
+    <t>1/555</t>
+  </si>
+  <si>
+    <t>20.0</t>
   </si>
 </sst>
 </file>
@@ -404,7 +716,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -445,6 +757,914 @@
         <v>10</v>
       </c>
     </row>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H2" t="s">
+        <v>101</v>
+      </c>
+      <c r="I2" t="s">
+        <v>102</v>
+      </c>
+      <c r="J2" t="s">
+        <v>107</v>
+      </c>
+      <c r="K2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" t="s">
+        <v>100</v>
+      </c>
+      <c r="H3" t="s">
+        <v>101</v>
+      </c>
+      <c r="I3" t="s">
+        <v>103</v>
+      </c>
+      <c r="J3" t="s">
+        <v>108</v>
+      </c>
+      <c r="K3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" t="s">
+        <v>100</v>
+      </c>
+      <c r="H4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I4" t="s">
+        <v>103</v>
+      </c>
+      <c r="J4" t="s">
+        <v>108</v>
+      </c>
+      <c r="K4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F5" t="s">
+        <v>98</v>
+      </c>
+      <c r="G5" t="s">
+        <v>100</v>
+      </c>
+      <c r="H5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I5" t="s">
+        <v>102</v>
+      </c>
+      <c r="J5" t="s">
+        <v>107</v>
+      </c>
+      <c r="K5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" t="s">
+        <v>99</v>
+      </c>
+      <c r="G6" t="s">
+        <v>100</v>
+      </c>
+      <c r="H6" t="s">
+        <v>101</v>
+      </c>
+      <c r="I6" t="s">
+        <v>104</v>
+      </c>
+      <c r="J6" t="s">
+        <v>109</v>
+      </c>
+      <c r="K6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G7" t="s">
+        <v>100</v>
+      </c>
+      <c r="H7" t="s">
+        <v>101</v>
+      </c>
+      <c r="I7" t="s">
+        <v>102</v>
+      </c>
+      <c r="J7" t="s">
+        <v>110</v>
+      </c>
+      <c r="K7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" t="s">
+        <v>99</v>
+      </c>
+      <c r="G8" t="s">
+        <v>100</v>
+      </c>
+      <c r="H8" t="s">
+        <v>101</v>
+      </c>
+      <c r="I8" t="s">
+        <v>104</v>
+      </c>
+      <c r="J8" t="s">
+        <v>109</v>
+      </c>
+      <c r="K8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" t="s">
+        <v>90</v>
+      </c>
+      <c r="F9" t="s">
+        <v>99</v>
+      </c>
+      <c r="G9" t="s">
+        <v>100</v>
+      </c>
+      <c r="H9" t="s">
+        <v>101</v>
+      </c>
+      <c r="I9" t="s">
+        <v>104</v>
+      </c>
+      <c r="J9" t="s">
+        <v>109</v>
+      </c>
+      <c r="K9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" t="s">
+        <v>87</v>
+      </c>
+      <c r="F10" t="s">
+        <v>99</v>
+      </c>
+      <c r="G10" t="s">
+        <v>100</v>
+      </c>
+      <c r="H10" t="s">
+        <v>101</v>
+      </c>
+      <c r="I10" t="s">
+        <v>104</v>
+      </c>
+      <c r="J10" t="s">
+        <v>111</v>
+      </c>
+      <c r="K10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" t="s">
+        <v>87</v>
+      </c>
+      <c r="F11" t="s">
+        <v>99</v>
+      </c>
+      <c r="G11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H11" t="s">
+        <v>101</v>
+      </c>
+      <c r="I11" t="s">
+        <v>104</v>
+      </c>
+      <c r="J11" t="s">
+        <v>111</v>
+      </c>
+      <c r="K11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" t="s">
+        <v>87</v>
+      </c>
+      <c r="F12" t="s">
+        <v>99</v>
+      </c>
+      <c r="G12" t="s">
+        <v>100</v>
+      </c>
+      <c r="H12" t="s">
+        <v>101</v>
+      </c>
+      <c r="I12" t="s">
+        <v>104</v>
+      </c>
+      <c r="J12" t="s">
+        <v>107</v>
+      </c>
+      <c r="K12" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" t="s">
+        <v>87</v>
+      </c>
+      <c r="F13" t="s">
+        <v>98</v>
+      </c>
+      <c r="G13" t="s">
+        <v>100</v>
+      </c>
+      <c r="H13" t="s">
+        <v>101</v>
+      </c>
+      <c r="I13" t="s">
+        <v>102</v>
+      </c>
+      <c r="J13" t="s">
+        <v>107</v>
+      </c>
+      <c r="K13" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" t="s">
+        <v>87</v>
+      </c>
+      <c r="F14" t="s">
+        <v>98</v>
+      </c>
+      <c r="G14" t="s">
+        <v>100</v>
+      </c>
+      <c r="H14" t="s">
+        <v>101</v>
+      </c>
+      <c r="I14" t="s">
+        <v>102</v>
+      </c>
+      <c r="J14" t="s">
+        <v>107</v>
+      </c>
+      <c r="K14" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" t="s">
+        <v>91</v>
+      </c>
+      <c r="F15" t="s">
+        <v>99</v>
+      </c>
+      <c r="G15" t="s">
+        <v>100</v>
+      </c>
+      <c r="H15" t="s">
+        <v>101</v>
+      </c>
+      <c r="I15" t="s">
+        <v>104</v>
+      </c>
+      <c r="J15" t="s">
+        <v>109</v>
+      </c>
+      <c r="K15" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16" t="s">
+        <v>90</v>
+      </c>
+      <c r="F16" t="s">
+        <v>99</v>
+      </c>
+      <c r="G16" t="s">
+        <v>100</v>
+      </c>
+      <c r="H16" t="s">
+        <v>101</v>
+      </c>
+      <c r="I16" t="s">
+        <v>104</v>
+      </c>
+      <c r="J16" t="s">
+        <v>109</v>
+      </c>
+      <c r="K16" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" t="s">
+        <v>87</v>
+      </c>
+      <c r="F17" t="s">
+        <v>99</v>
+      </c>
+      <c r="G17" t="s">
+        <v>100</v>
+      </c>
+      <c r="H17" t="s">
+        <v>101</v>
+      </c>
+      <c r="I17" t="s">
+        <v>104</v>
+      </c>
+      <c r="J17" t="s">
+        <v>107</v>
+      </c>
+      <c r="K17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" t="s">
+        <v>100</v>
+      </c>
+      <c r="H18" t="s">
+        <v>101</v>
+      </c>
+      <c r="I18" t="s">
+        <v>105</v>
+      </c>
+      <c r="J18" t="s">
+        <v>108</v>
+      </c>
+      <c r="K18" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" t="s">
+        <v>49</v>
+      </c>
+      <c r="G19" t="s">
+        <v>100</v>
+      </c>
+      <c r="H19" t="s">
+        <v>101</v>
+      </c>
+      <c r="I19" t="s">
+        <v>106</v>
+      </c>
+      <c r="J19" t="s">
+        <v>112</v>
+      </c>
+      <c r="K19" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" t="s">
+        <v>92</v>
+      </c>
+      <c r="F20" t="s">
+        <v>99</v>
+      </c>
+      <c r="G20" t="s">
+        <v>100</v>
+      </c>
+      <c r="H20" t="s">
+        <v>101</v>
+      </c>
+      <c r="I20" t="s">
+        <v>104</v>
+      </c>
+      <c r="J20" t="s">
+        <v>108</v>
+      </c>
+      <c r="K20" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" t="s">
+        <v>93</v>
+      </c>
+      <c r="F21" t="s">
+        <v>99</v>
+      </c>
+      <c r="G21" t="s">
+        <v>100</v>
+      </c>
+      <c r="H21" t="s">
+        <v>101</v>
+      </c>
+      <c r="I21" t="s">
+        <v>104</v>
+      </c>
+      <c r="J21" t="s">
+        <v>108</v>
+      </c>
+      <c r="K21" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" t="s">
+        <v>83</v>
+      </c>
+      <c r="E22" t="s">
+        <v>94</v>
+      </c>
+      <c r="F22" t="s">
+        <v>99</v>
+      </c>
+      <c r="G22" t="s">
+        <v>100</v>
+      </c>
+      <c r="H22" t="s">
+        <v>101</v>
+      </c>
+      <c r="I22" t="s">
+        <v>104</v>
+      </c>
+      <c r="J22" t="s">
+        <v>108</v>
+      </c>
+      <c r="K22" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" t="s">
+        <v>84</v>
+      </c>
+      <c r="E23" t="s">
+        <v>95</v>
+      </c>
+      <c r="F23" t="s">
+        <v>99</v>
+      </c>
+      <c r="G23" t="s">
+        <v>100</v>
+      </c>
+      <c r="H23" t="s">
+        <v>101</v>
+      </c>
+      <c r="I23" t="s">
+        <v>105</v>
+      </c>
+      <c r="J23" t="s">
+        <v>111</v>
+      </c>
+      <c r="K23" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" t="s">
+        <v>85</v>
+      </c>
+      <c r="E24" t="s">
+        <v>96</v>
+      </c>
+      <c r="F24" t="s">
+        <v>99</v>
+      </c>
+      <c r="G24" t="s">
+        <v>100</v>
+      </c>
+      <c r="H24" t="s">
+        <v>101</v>
+      </c>
+      <c r="I24" t="s">
+        <v>104</v>
+      </c>
+      <c r="J24" t="s">
+        <v>113</v>
+      </c>
+      <c r="K24" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" t="s">
+        <v>53</v>
+      </c>
+      <c r="G25" t="s">
+        <v>100</v>
+      </c>
+      <c r="H25" t="s">
+        <v>101</v>
+      </c>
+      <c r="I25" t="s">
+        <v>106</v>
+      </c>
+      <c r="J25" t="s">
+        <v>112</v>
+      </c>
+      <c r="K25" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" t="s">
+        <v>54</v>
+      </c>
+      <c r="G26" t="s">
+        <v>100</v>
+      </c>
+      <c r="H26" t="s">
+        <v>101</v>
+      </c>
+      <c r="I26" t="s">
+        <v>104</v>
+      </c>
+      <c r="J26" t="s">
+        <v>111</v>
+      </c>
+      <c r="K26" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" t="s">
+        <v>62</v>
+      </c>
+      <c r="D27" t="s">
+        <v>82</v>
+      </c>
+      <c r="E27" t="s">
+        <v>93</v>
+      </c>
+      <c r="F27" t="s">
+        <v>99</v>
+      </c>
+      <c r="G27" t="s">
+        <v>100</v>
+      </c>
+      <c r="H27" t="s">
+        <v>101</v>
+      </c>
+      <c r="I27" t="s">
+        <v>104</v>
+      </c>
+      <c r="J27" t="s">
+        <v>108</v>
+      </c>
+      <c r="K27" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28" t="s">
+        <v>86</v>
+      </c>
+      <c r="E28" t="s">
+        <v>97</v>
+      </c>
+      <c r="F28" t="s">
+        <v>99</v>
+      </c>
+      <c r="G28" t="s">
+        <v>100</v>
+      </c>
+      <c r="H28" t="s">
+        <v>101</v>
+      </c>
+      <c r="I28" t="s">
+        <v>104</v>
+      </c>
+      <c r="J28" t="s">
+        <v>109</v>
+      </c>
+      <c r="K28" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" t="s">
+        <v>75</v>
+      </c>
+      <c r="E29" t="s">
+        <v>87</v>
+      </c>
+      <c r="F29" t="s">
+        <v>99</v>
+      </c>
+      <c r="G29" t="s">
+        <v>100</v>
+      </c>
+      <c r="H29" t="s">
+        <v>101</v>
+      </c>
+      <c r="I29" t="s">
+        <v>104</v>
+      </c>
+      <c r="J29" t="s">
+        <v>109</v>
+      </c>
+      <c r="K29" t="s">
+        <v>114</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
modellverwaltungs btn mit reset auf backup
</commit_message>
<xml_diff>
--- a/models/stashedTrainData.XLSX
+++ b/models/stashedTrainData.XLSX
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="79">
   <si>
     <t>Produktmerkmal</t>
   </si>
@@ -49,12 +49,6 @@
     <t>Lenkungsmethode</t>
   </si>
   <si>
-    <t>280</t>
-  </si>
-  <si>
-    <t>290</t>
-  </si>
-  <si>
     <t>300</t>
   </si>
   <si>
@@ -103,54 +97,45 @@
     <t>1020</t>
   </si>
   <si>
-    <t>Rautiefe</t>
+    <t>Bohrungstiefe</t>
+  </si>
+  <si>
+    <t>Rundlauf</t>
+  </si>
+  <si>
+    <t>Innen-ø33,46</t>
+  </si>
+  <si>
+    <t>Innen-ø33,6H6</t>
+  </si>
+  <si>
+    <t>Innen-ø33,6</t>
+  </si>
+  <si>
+    <t>Abstand</t>
+  </si>
+  <si>
+    <t>Aussen-ø37,4</t>
+  </si>
+  <si>
+    <t>Drehm.</t>
+  </si>
+  <si>
+    <t>Rolliertiefe</t>
+  </si>
+  <si>
+    <t>Sichtprüfung</t>
   </si>
   <si>
     <t>Bohrungs-ø</t>
   </si>
   <si>
-    <t>Bohrungstiefe</t>
-  </si>
-  <si>
-    <t>Rundlauf</t>
-  </si>
-  <si>
-    <t>Innen-ø33,46</t>
-  </si>
-  <si>
-    <t>Innen-ø33,6H6</t>
-  </si>
-  <si>
-    <t>Innen-ø33,6</t>
-  </si>
-  <si>
-    <t>Abstand</t>
-  </si>
-  <si>
-    <t>Aussen-ø37,4</t>
-  </si>
-  <si>
-    <t>Drehm.</t>
-  </si>
-  <si>
-    <t>Rolliertiefe</t>
-  </si>
-  <si>
-    <t>Sichtprüfung</t>
-  </si>
-  <si>
     <t>Maschinenabnahme</t>
   </si>
   <si>
     <t>siehe</t>
   </si>
   <si>
-    <t>0,000 µm</t>
-  </si>
-  <si>
-    <t>9,000 mm</t>
-  </si>
-  <si>
     <t>1,000 mm</t>
   </si>
   <si>
@@ -175,12 +160,6 @@
     <t>35,000 mm</t>
   </si>
   <si>
-    <t>25.0</t>
-  </si>
-  <si>
-    <t>9.0</t>
-  </si>
-  <si>
     <t>1.2</t>
   </si>
   <si>
@@ -208,15 +187,12 @@
     <t>0.05</t>
   </si>
   <si>
+    <t>1.0</t>
+  </si>
+  <si>
     <t>0.0</t>
   </si>
   <si>
-    <t>8.9</t>
-  </si>
-  <si>
-    <t>1.0</t>
-  </si>
-  <si>
     <t>33.604</t>
   </si>
   <si>
@@ -235,9 +211,6 @@
     <t>34.8</t>
   </si>
   <si>
-    <t>µm</t>
-  </si>
-  <si>
     <t>mm</t>
   </si>
   <si>
@@ -247,9 +220,6 @@
     <t>MS40-MGH</t>
   </si>
   <si>
-    <t>Rauhigkeitsmessgerät</t>
-  </si>
-  <si>
     <t>MESSUHR</t>
   </si>
   <si>
@@ -262,10 +232,10 @@
     <t>visuelle Prüfung</t>
   </si>
   <si>
+    <t>2/20</t>
+  </si>
+  <si>
     <t>1/444</t>
-  </si>
-  <si>
-    <t>2/20</t>
   </si>
   <si>
     <t>1/1</t>
@@ -638,7 +608,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -684,34 +654,34 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="F2" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="G2" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="H2" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="I2" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="J2" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="K2" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -719,34 +689,34 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" t="s">
         <v>65</v>
       </c>
-      <c r="F3" t="s">
-        <v>74</v>
-      </c>
       <c r="G3" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="H3" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="I3" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="J3" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="K3" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -754,34 +724,22 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H4" t="s">
+        <v>67</v>
+      </c>
+      <c r="I4" t="s">
+        <v>69</v>
+      </c>
+      <c r="J4" t="s">
         <v>74</v>
       </c>
-      <c r="G4" t="s">
-        <v>75</v>
-      </c>
-      <c r="H4" t="s">
-        <v>76</v>
-      </c>
-      <c r="I4" t="s">
-        <v>78</v>
-      </c>
-      <c r="J4" t="s">
-        <v>83</v>
-      </c>
       <c r="K4" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -789,34 +747,22 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F5" t="s">
-        <v>74</v>
+        <v>30</v>
       </c>
       <c r="G5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H5" t="s">
+        <v>67</v>
+      </c>
+      <c r="I5" t="s">
+        <v>70</v>
+      </c>
+      <c r="J5" t="s">
         <v>75</v>
       </c>
-      <c r="H5" t="s">
-        <v>76</v>
-      </c>
-      <c r="I5" t="s">
-        <v>78</v>
-      </c>
-      <c r="J5" t="s">
-        <v>82</v>
-      </c>
       <c r="K5" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -824,22 +770,34 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" t="s">
+        <v>65</v>
       </c>
       <c r="G6" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="H6" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="I6" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="J6" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="K6" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -847,22 +805,34 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" t="s">
+        <v>65</v>
       </c>
       <c r="G7" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="H7" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="I7" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="J7" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="K7" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -870,34 +840,34 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E8" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="F8" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8" t="s">
+        <v>66</v>
+      </c>
+      <c r="H8" t="s">
+        <v>67</v>
+      </c>
+      <c r="I8" t="s">
+        <v>68</v>
+      </c>
+      <c r="J8" t="s">
         <v>74</v>
       </c>
-      <c r="G8" t="s">
-        <v>75</v>
-      </c>
-      <c r="H8" t="s">
-        <v>76</v>
-      </c>
-      <c r="I8" t="s">
-        <v>78</v>
-      </c>
-      <c r="J8" t="s">
-        <v>84</v>
-      </c>
       <c r="K8" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -905,34 +875,34 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D9" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E9" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F9" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="G9" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="H9" t="s">
+        <v>67</v>
+      </c>
+      <c r="I9" t="s">
+        <v>69</v>
+      </c>
+      <c r="J9" t="s">
         <v>76</v>
       </c>
-      <c r="I9" t="s">
-        <v>78</v>
-      </c>
-      <c r="J9" t="s">
-        <v>84</v>
-      </c>
       <c r="K9" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -940,34 +910,34 @@
         <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D10" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E10" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="G10" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="H10" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="I10" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="J10" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="K10" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -975,34 +945,22 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" t="s">
+        <v>66</v>
+      </c>
+      <c r="H11" t="s">
+        <v>67</v>
+      </c>
+      <c r="I11" t="s">
         <v>70</v>
       </c>
-      <c r="F11" t="s">
-        <v>74</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="J11" t="s">
         <v>75</v>
       </c>
-      <c r="H11" t="s">
-        <v>76</v>
-      </c>
-      <c r="I11" t="s">
-        <v>79</v>
-      </c>
-      <c r="J11" t="s">
-        <v>86</v>
-      </c>
       <c r="K11" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1010,34 +968,22 @@
         <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" t="s">
-        <v>61</v>
-      </c>
-      <c r="E12" t="s">
-        <v>71</v>
-      </c>
-      <c r="F12" t="s">
-        <v>74</v>
+        <v>36</v>
       </c>
       <c r="G12" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="H12" t="s">
+        <v>67</v>
+      </c>
+      <c r="I12" t="s">
+        <v>68</v>
+      </c>
+      <c r="J12" t="s">
         <v>76</v>
       </c>
-      <c r="I12" t="s">
-        <v>78</v>
-      </c>
-      <c r="J12" t="s">
-        <v>87</v>
-      </c>
       <c r="K12" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1045,22 +991,34 @@
         <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" t="s">
+        <v>60</v>
+      </c>
+      <c r="F13" t="s">
+        <v>65</v>
       </c>
       <c r="G13" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="H13" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="I13" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="J13" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="K13" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1068,22 +1026,34 @@
         <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" t="s">
+        <v>65</v>
       </c>
       <c r="G14" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="H14" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="I14" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="J14" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="K14" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1091,34 +1061,34 @@
         <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" t="s">
         <v>58</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15" t="s">
+        <v>66</v>
+      </c>
+      <c r="H15" t="s">
+        <v>67</v>
+      </c>
+      <c r="I15" t="s">
         <v>68</v>
       </c>
-      <c r="F15" t="s">
-        <v>74</v>
-      </c>
-      <c r="G15" t="s">
-        <v>75</v>
-      </c>
-      <c r="H15" t="s">
-        <v>76</v>
-      </c>
-      <c r="I15" t="s">
-        <v>78</v>
-      </c>
       <c r="J15" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="K15" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1126,34 +1096,22 @@
         <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" t="s">
-        <v>62</v>
-      </c>
-      <c r="E16" t="s">
-        <v>72</v>
-      </c>
-      <c r="F16" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" t="s">
+        <v>66</v>
+      </c>
+      <c r="H16" t="s">
+        <v>67</v>
+      </c>
+      <c r="I16" t="s">
+        <v>71</v>
+      </c>
+      <c r="J16" t="s">
         <v>74</v>
       </c>
-      <c r="G16" t="s">
-        <v>75</v>
-      </c>
-      <c r="H16" t="s">
-        <v>76</v>
-      </c>
-      <c r="I16" t="s">
-        <v>78</v>
-      </c>
-      <c r="J16" t="s">
-        <v>83</v>
-      </c>
       <c r="K16" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1161,172 +1119,114 @@
         <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" t="s">
-        <v>63</v>
-      </c>
-      <c r="E17" t="s">
-        <v>64</v>
-      </c>
-      <c r="F17" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" t="s">
+        <v>66</v>
+      </c>
+      <c r="H17" t="s">
+        <v>67</v>
+      </c>
+      <c r="I17" t="s">
+        <v>71</v>
+      </c>
+      <c r="J17" t="s">
         <v>74</v>
       </c>
-      <c r="G17" t="s">
-        <v>75</v>
-      </c>
-      <c r="H17" t="s">
-        <v>76</v>
-      </c>
-      <c r="I17" t="s">
-        <v>78</v>
-      </c>
-      <c r="J17" t="s">
-        <v>83</v>
-      </c>
       <c r="K17" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="G18" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="H18" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="I18" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="J18" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="K18" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="G19" t="s">
+        <v>66</v>
+      </c>
+      <c r="H19" t="s">
+        <v>67</v>
+      </c>
+      <c r="I19" t="s">
+        <v>70</v>
+      </c>
+      <c r="J19" t="s">
         <v>75</v>
       </c>
-      <c r="H19" t="s">
-        <v>76</v>
-      </c>
-      <c r="I19" t="s">
-        <v>81</v>
-      </c>
-      <c r="J19" t="s">
-        <v>84</v>
-      </c>
       <c r="K19" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G20" t="s">
+        <v>66</v>
+      </c>
+      <c r="H20" t="s">
+        <v>67</v>
+      </c>
+      <c r="I20" t="s">
+        <v>70</v>
+      </c>
+      <c r="J20" t="s">
         <v>75</v>
       </c>
-      <c r="H20" t="s">
-        <v>76</v>
-      </c>
-      <c r="I20" t="s">
-        <v>79</v>
-      </c>
-      <c r="J20" t="s">
-        <v>84</v>
-      </c>
       <c r="K20" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G21" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="H21" t="s">
+        <v>67</v>
+      </c>
+      <c r="I21" t="s">
+        <v>68</v>
+      </c>
+      <c r="J21" t="s">
         <v>76</v>
       </c>
-      <c r="I21" t="s">
-        <v>80</v>
-      </c>
-      <c r="J21" t="s">
-        <v>85</v>
-      </c>
       <c r="K21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" t="s">
-        <v>39</v>
-      </c>
-      <c r="G22" t="s">
-        <v>75</v>
-      </c>
-      <c r="H22" t="s">
-        <v>76</v>
-      </c>
-      <c r="I22" t="s">
-        <v>80</v>
-      </c>
-      <c r="J22" t="s">
-        <v>85</v>
-      </c>
-      <c r="K22" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
-      <c r="A23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" t="s">
-        <v>40</v>
-      </c>
-      <c r="G23" t="s">
-        <v>75</v>
-      </c>
-      <c r="H23" t="s">
-        <v>76</v>
-      </c>
-      <c r="I23" t="s">
-        <v>78</v>
-      </c>
-      <c r="J23" t="s">
-        <v>86</v>
-      </c>
-      <c r="K23" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>